<commit_message>
update timekeeping api to download
</commit_message>
<xml_diff>
--- a/app/data/input_file6.xlsx
+++ b/app/data/input_file6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="17160"/>
+    <workbookView windowWidth="24460" windowHeight="11560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1109,8 +1109,8 @@
   </sheetPr>
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>

</xml_diff>